<commit_message>
added urls for emails
</commit_message>
<xml_diff>
--- a/unique_pairs.xlsx
+++ b/unique_pairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheoryDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16040734-B921-45DB-9F36-7E0F80EE0765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC13FFF-81DC-424D-AC9E-465C4AA0F48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0EDC7369-C9CA-4FF7-AB75-E2D252A4F451}"/>
+    <workbookView xWindow="-16320" yWindow="-6840" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{0EDC7369-C9CA-4FF7-AB75-E2D252A4F451}"/>
   </bookViews>
   <sheets>
     <sheet name="allWithCat" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="340">
   <si>
     <t>pattern</t>
   </si>
@@ -1031,6 +1031,33 @@
   </si>
   <si>
     <t>test statistic</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/dev@cassandra.apache.org/msg08188.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/dev@cassandra.apache.org/msg15537.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/dev@cassandra.apache.org/msg16516.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/hadoop-dev@lucene.apache.org/msg02047.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/yarn-dev@hadoop.apache.org/msg00935.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/hdfs-dev@hadoop.apache.org/msg14116.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/hdfs-dev@hadoop.apache.org/msg36082.html</t>
+  </si>
+  <si>
+    <t>https://www.mail-archive.com/dev@cassandra.apache.org/msg07951.html</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -6241,15 +6268,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BDCCC6-FAD5-4A27-9097-43EF76A0C037}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -6268,8 +6295,11 @@
       <c r="H1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>25115</v>
       </c>
@@ -6288,8 +6318,11 @@
       <c r="H2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>39747</v>
       </c>
@@ -6308,8 +6341,11 @@
       <c r="H3" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>41099</v>
       </c>
@@ -6328,8 +6364,11 @@
       <c r="H4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>398</v>
       </c>
@@ -6348,8 +6387,11 @@
       <c r="H5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>15549</v>
       </c>
@@ -6368,8 +6410,11 @@
       <c r="H6" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>21234</v>
       </c>
@@ -6388,8 +6433,11 @@
       <c r="H7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>36643</v>
       </c>
@@ -6408,8 +6456,11 @@
       <c r="H8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>24379</v>
       </c>
@@ -6428,9 +6479,13 @@
       <c r="H9" t="s">
         <v>177</v>
       </c>
+      <c r="K9" t="s">
+        <v>338</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6438,7 +6493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4A8668-F27C-49AC-A0DA-7EF6B7F9D0EB}">
   <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>